<commit_message>
Promedio avance de SOE - CP
</commit_message>
<xml_diff>
--- a/Desarrollo/SOE/Gestion/SOE - CP.xlsx
+++ b/Desarrollo/SOE/Gestion/SOE - CP.xlsx
@@ -886,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q1017"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1331,7 +1331,7 @@
         <v>38</v>
       </c>
       <c r="Q17" s="15">
-        <v>0.4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
@@ -1357,7 +1357,7 @@
         <v>29</v>
       </c>
       <c r="Q18" s="15">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
@@ -1383,7 +1383,7 @@
         <v>38</v>
       </c>
       <c r="Q19" s="15">
-        <v>0.3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
@@ -1559,7 +1559,7 @@
         <v>97</v>
       </c>
       <c r="Q26" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
@@ -1611,7 +1611,7 @@
         <v>50</v>
       </c>
       <c r="Q28" s="16">
-        <v>0.72719999999999996</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="29" spans="2:17" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -2042,9 +2042,7 @@
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
       <c r="P46" s="5"/>
-      <c r="Q46" s="15">
-        <v>0</v>
-      </c>
+      <c r="Q46" s="15"/>
     </row>
     <row r="47" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="10" t="s">
@@ -2196,9 +2194,7 @@
       <c r="N52" s="29"/>
       <c r="O52" s="28"/>
       <c r="P52" s="28"/>
-      <c r="Q52" s="15">
-        <v>0</v>
-      </c>
+      <c r="Q52" s="15"/>
     </row>
     <row r="53" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="47" t="s">
@@ -2218,9 +2214,7 @@
       <c r="N53" s="27"/>
       <c r="O53" s="27"/>
       <c r="P53" s="27"/>
-      <c r="Q53" s="15">
-        <v>0</v>
-      </c>
+      <c r="Q53" s="15"/>
     </row>
     <row r="54" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="33" t="s">
@@ -2318,9 +2312,7 @@
       <c r="N57" s="27"/>
       <c r="O57" s="27"/>
       <c r="P57" s="56"/>
-      <c r="Q57" s="15">
-        <v>0</v>
-      </c>
+      <c r="Q57" s="15"/>
     </row>
     <row r="58" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="37" t="s">
@@ -2366,9 +2358,7 @@
       <c r="N59" s="27"/>
       <c r="O59" s="27"/>
       <c r="P59" s="56"/>
-      <c r="Q59" s="15">
-        <v>0</v>
-      </c>
+      <c r="Q59" s="15"/>
     </row>
     <row r="60" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="39" t="s">
@@ -2440,14 +2430,12 @@
       <c r="N62" s="27"/>
       <c r="O62" s="27"/>
       <c r="P62" s="56"/>
-      <c r="Q62" s="15">
-        <v>0</v>
-      </c>
+      <c r="Q62" s="15"/>
     </row>
     <row r="63" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q63" s="62">
         <f>AVERAGE(Q8:Q62)</f>
-        <v>0.41161333333333344</v>
+        <v>0.54116410256410252</v>
       </c>
     </row>
     <row r="64" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Actualizacion de Cronograma de Proyecto
</commit_message>
<xml_diff>
--- a/Desarrollo/SOE/Gestion/SOE - CP.xlsx
+++ b/Desarrollo/SOE/Gestion/SOE - CP.xlsx
@@ -904,7 +904,7 @@
   <dimension ref="B1:Q1019"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B49" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="R62" sqref="R62"/>
+      <selection activeCell="R61" sqref="R61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1808,7 +1808,7 @@
         <v>53</v>
       </c>
       <c r="Q36" s="15">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.25">
@@ -1834,7 +1834,7 @@
         <v>53</v>
       </c>
       <c r="Q37" s="15">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.25">
@@ -1860,7 +1860,7 @@
         <v>53</v>
       </c>
       <c r="Q38" s="15">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="2:17" s="63" customFormat="1" x14ac:dyDescent="0.25">
@@ -1886,7 +1886,7 @@
         <v>53</v>
       </c>
       <c r="Q39" s="15">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="2:17" s="63" customFormat="1" x14ac:dyDescent="0.25">
@@ -1912,7 +1912,7 @@
         <v>53</v>
       </c>
       <c r="Q40" s="15">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.25">
@@ -2308,7 +2308,7 @@
         <v>59</v>
       </c>
       <c r="Q56" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2406,7 +2406,7 @@
         <v>61</v>
       </c>
       <c r="Q60" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2452,7 +2452,7 @@
         <v>70</v>
       </c>
       <c r="Q62" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2478,7 +2478,7 @@
         <v>59</v>
       </c>
       <c r="Q63" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2504,7 +2504,7 @@
     <row r="65" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q65" s="62">
         <f>AVERAGE(Q8:Q64)</f>
-        <v>0.79268292682926833</v>
+        <v>0.95121951219512191</v>
       </c>
     </row>
     <row r="66" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>